<commit_message>
BFA - all master data
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/blacklisted_words.xlsx
+++ b/mosip_master/xlsx/blacklisted_words.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Balaji.Alluru\Desktop\Mosip\GitHub\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Office\codes\bfa\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="1092" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>lang_code</t>
   </si>
@@ -38,27 +38,6 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>eng</t>
-  </si>
-  <si>
-    <t>shit</t>
-  </si>
-  <si>
-    <t>Blacklisted Word</t>
-  </si>
-  <si>
-    <t>TRUE</t>
-  </si>
-  <si>
-    <t>damn</t>
-  </si>
-  <si>
-    <t>nigga</t>
-  </si>
-  <si>
-    <t>dammit</t>
-  </si>
-  <si>
     <t>fra</t>
   </si>
   <si>
@@ -69,27 +48,12 @@
   </si>
   <si>
     <t>bon sang</t>
-  </si>
-  <si>
-    <t>ara</t>
-  </si>
-  <si>
-    <t>القرف</t>
-  </si>
-  <si>
-    <t>كلمة في القائمة السوداء</t>
-  </si>
-  <si>
-    <t>اللعنة</t>
-  </si>
-  <si>
-    <t>نيغا</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -436,17 +400,17 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -460,139 +424,76 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D11"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D12"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D13"/>
     </row>
   </sheetData>

</xml_diff>